<commit_message>
Added more multithreading questions
Added more multithreading questions
</commit_message>
<xml_diff>
--- a/src/com/corejava/practice/topics/CoreJavaTopicsOrQuestions.xlsx
+++ b/src/com/corejava/practice/topics/CoreJavaTopicsOrQuestions.xlsx
@@ -12,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CoreJavaTopicsOrQuestions!$A$1:$C$34</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
   <si>
     <t>Topic</t>
   </si>
@@ -170,6 +170,33 @@
   </si>
   <si>
     <t>What is contex-switching in multi threading?</t>
+  </si>
+  <si>
+    <t>How can we make sure main is the last thread to finish java program?</t>
+  </si>
+  <si>
+    <t>How does thread communicate with each other?</t>
+  </si>
+  <si>
+    <t>Why wait(), notify() and notifyAll() methods are in Object class?</t>
+  </si>
+  <si>
+    <t>Why we call wait(), notify() and notifyAll() methods have to be called from synchronized method or block?</t>
+  </si>
+  <si>
+    <t>Why sleep() and yeild() methods are static?</t>
+  </si>
+  <si>
+    <t>Difference between interrupted() and isInterrupted() method.</t>
+  </si>
+  <si>
+    <t>How can we achieve thread safty in java?</t>
+  </si>
+  <si>
+    <t>Which is more preferred, synchronized method or block?</t>
+  </si>
+  <si>
+    <t>What is ThreadLocal?</t>
   </si>
 </sst>
 </file>
@@ -1014,11 +1041,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1317,6 +1344,78 @@
         <v>50</v>
       </c>
     </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C34"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated with new questions and answer links
</commit_message>
<xml_diff>
--- a/src/com/corejava/practice/topics/CoreJavaTopicsOrQuestions.xlsx
+++ b/src/com/corejava/practice/topics/CoreJavaTopicsOrQuestions.xlsx
@@ -10,14 +10,14 @@
     <sheet name="CoreJavaTopicsOrQuestions" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CoreJavaTopicsOrQuestions!$A$1:$C$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CoreJavaTopicsOrQuestions!$A$1:$C$43</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="73">
   <si>
     <t>Topic</t>
   </si>
@@ -76,9 +76,6 @@
     <t>https://www.math.uni-hamburg.de/doc/java/jdk1.4.1/docs/guide/serialization/spec/input.doc7.html</t>
   </si>
   <si>
-    <t>What is the difference between Serializable and Externalizable class?</t>
-  </si>
-  <si>
     <t>ObjectCreation</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>What is Runnable and Callable?</t>
   </si>
   <si>
-    <t>Can we declare a constructor static? Explain your answer why.</t>
-  </si>
-  <si>
     <t>Can we declare outer class static? Explain your answer why.</t>
   </si>
   <si>
@@ -197,13 +191,58 @@
   </si>
   <si>
     <t>What is ThreadLocal?</t>
+  </si>
+  <si>
+    <t>How Java works?</t>
+  </si>
+  <si>
+    <t>https://javarevisited.blogspot.com/2012/12/how-classloader-works-in-java.html</t>
+  </si>
+  <si>
+    <t>https://javarevisited.blogspot.com/2011/01/how-classpath-work-in-java.html</t>
+  </si>
+  <si>
+    <t>What is the difference between ClassNotFoundException and NoClassDefFoundError?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=sjMe9aecW_A</t>
+  </si>
+  <si>
+    <t>What is the difference between poll() and peek() method?</t>
+  </si>
+  <si>
+    <t>What is race condition?</t>
+  </si>
+  <si>
+    <t>How to avoid dead lock?</t>
+  </si>
+  <si>
+    <t>https://javarevisited.blogspot.com/2018/08/how-to-avoid-deadlock-in-java-threads.html</t>
+  </si>
+  <si>
+    <t>Why can't we make top level class as static?</t>
+  </si>
+  <si>
+    <t>What is Future object in java?</t>
+  </si>
+  <si>
+    <t>https://www.interviewsansar.com/2018/03/24/loose-coupling-and-tight-coupling-in-java/</t>
+  </si>
+  <si>
+    <t>https://www.java67.com/2018/07/java-enum-with-constructor-example.html?m=1</t>
+  </si>
+  <si>
+    <t>What is the difference between Serializable and Externalizable interface?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,6 +377,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -658,7 +704,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -701,13 +747,18 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -741,6 +792,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1041,11 +1093,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1072,6 +1124,9 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
@@ -1080,6 +1135,9 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
@@ -1088,6 +1146,9 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
@@ -1096,6 +1157,9 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
@@ -1154,23 +1218,26 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
         <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="B13" t="s">
-        <v>23</v>
+      <c r="C13" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1178,15 +1245,18 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
         <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1194,7 +1264,7 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1202,95 +1272,95 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
         <v>29</v>
-      </c>
-      <c r="B19" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
         <v>32</v>
-      </c>
-      <c r="B21" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1298,127 +1368,193 @@
         <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" t="s">
         <v>45</v>
-      </c>
-      <c r="B31" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>25</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
-        <v>25</v>
-      </c>
-      <c r="B35" t="s">
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s">
-        <v>25</v>
-      </c>
-      <c r="B37" t="s">
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
-        <v>25</v>
-      </c>
-      <c r="B38" t="s">
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" t="s">
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
-        <v>25</v>
-      </c>
-      <c r="B40" t="s">
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" t="s">
-        <v>25</v>
-      </c>
-      <c r="B41" t="s">
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="C43" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" t="s">
-        <v>25</v>
-      </c>
-      <c r="B43" t="s">
-        <v>59</v>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C34"/>
+  <autoFilter ref="A1:C43"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C45" r:id="rId3"/>
+    <hyperlink ref="C43" r:id="rId4"/>
+    <hyperlink ref="C48" r:id="rId5"/>
+    <hyperlink ref="C14" r:id="rId6"/>
+    <hyperlink ref="C13" r:id="rId7"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>